<commit_message>
Update Kopie von DatenbankSchraube.xlsx
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint2/Sprint2/Kopie von DatenbankSchraube.xlsx
+++ b/Sprint 2/Sprint2/Sprint2/Kopie von DatenbankSchraube.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wurbs\Documents\Uni\Hsp\HSP_GruppeF_Sprint1\Sprint 2\Sprint2\Sprint2\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wurbs\Documents\Uni\Hsp\HSP_GruppeF_Sprint1\Sprint 2\Sprint2\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72737085-6F0C-4FBB-8474-CD1BE2DF256D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{162E65F2-6127-49F1-95E7-2BE99963E31D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1935" windowWidth="20520" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Sechskantschraube</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>dk</t>
+  </si>
+  <si>
+    <t>Senkschraube innensechskant</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -169,6 +172,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -177,7 +189,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
@@ -189,8 +201,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -476,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -487,17 +507,22 @@
     <col min="1" max="1" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="K1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -522,8 +547,20 @@
       <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -548,8 +585,20 @@
       <c r="I3" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K3" s="10">
+        <v>3</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2</v>
+      </c>
+      <c r="M3" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="N3" s="10">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -574,8 +623,20 @@
       <c r="I4" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K4" s="11">
+        <v>4</v>
+      </c>
+      <c r="L4" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="N4" s="11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -600,8 +661,20 @@
       <c r="I5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K5" s="10">
+        <v>5</v>
+      </c>
+      <c r="L5" s="10">
+        <v>3</v>
+      </c>
+      <c r="M5" s="10">
+        <v>9.4</v>
+      </c>
+      <c r="N5" s="10">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>6</v>
       </c>
@@ -626,8 +699,20 @@
       <c r="I6" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K6" s="11">
+        <v>6</v>
+      </c>
+      <c r="L6" s="11">
+        <v>4</v>
+      </c>
+      <c r="M6" s="11">
+        <v>11.3</v>
+      </c>
+      <c r="N6" s="11">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>8</v>
       </c>
@@ -652,8 +737,20 @@
       <c r="I7" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K7" s="10">
+        <v>8</v>
+      </c>
+      <c r="L7" s="10">
+        <v>5</v>
+      </c>
+      <c r="M7" s="10">
+        <v>15.2</v>
+      </c>
+      <c r="N7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>10</v>
       </c>
@@ -678,8 +775,20 @@
       <c r="I8" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K8" s="11">
+        <v>10</v>
+      </c>
+      <c r="L8" s="11">
+        <v>6</v>
+      </c>
+      <c r="M8" s="11">
+        <v>19.2</v>
+      </c>
+      <c r="N8" s="11">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>12</v>
       </c>
@@ -704,8 +813,20 @@
       <c r="I9" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K9" s="10">
+        <v>12</v>
+      </c>
+      <c r="L9" s="10">
+        <v>8</v>
+      </c>
+      <c r="M9" s="10">
+        <v>23.1</v>
+      </c>
+      <c r="N9" s="10">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>14</v>
       </c>
@@ -730,8 +851,20 @@
       <c r="I10" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K10" s="11">
+        <v>16</v>
+      </c>
+      <c r="L10" s="11">
+        <v>10</v>
+      </c>
+      <c r="M10" s="11">
+        <v>29</v>
+      </c>
+      <c r="N10" s="11">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>16</v>
       </c>
@@ -756,8 +889,20 @@
       <c r="I11" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K11" s="10">
+        <v>20</v>
+      </c>
+      <c r="L11" s="10">
+        <v>12</v>
+      </c>
+      <c r="M11" s="10">
+        <v>36</v>
+      </c>
+      <c r="N11" s="10">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -783,7 +928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>24</v>
       </c>
@@ -809,7 +954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -835,7 +980,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>36</v>
       </c>
@@ -850,8 +995,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>